<commit_message>
test change in directory
</commit_message>
<xml_diff>
--- a/SIMPOM directory.xlsx
+++ b/SIMPOM directory.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Ontology IRI</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>https://github.com/arsarkar/SIMPOM/blob/master/impm-ind%24001.owl</t>
+  </si>
+  <si>
+    <t>Test Onotlogy</t>
   </si>
 </sst>
 </file>
@@ -98,7 +101,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -158,11 +161,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -174,6 +188,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -477,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,6 +574,11 @@
       </c>
       <c r="D5" s="4"/>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>